<commit_message>
ajout des films festival au json - lab
</commit_message>
<xml_diff>
--- a/Programme.json_builder/work/enriched.xlsx
+++ b/Programme.json_builder/work/enriched.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U24"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,7 +543,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2025-02-04</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Le temps des moissons</t>
+          <t>La vie après Siham</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -564,91 +564,83 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Huo Meng</t>
+          <t>Namir Abdel Messeeh</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Ours d'argent meilleure réalisation Berlin 2025</t>
+          <t>Invité ADRC Cédric Lépine - Partenariat ADRC</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Coup de cœur</t>
-        </is>
-      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>https://fr.web.img6.acsta.net/c_310_420/img/74/0e/740e757ee905b05882b204567f5ea1b9.jpg</t>
+          <t>https://fr.web.img6.acsta.net/c_310_420/img/38/18/38181f1fe67de6a511e5a075587f98a6.jpg</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Chuang doit passer l’année de ses dix ans à la campagne, en famille mais sans ses parents, partis en ville chercher du travail. Le cycle des saisons, des mariages et des funérailles, le poids des traditions et l’attrait du progrès, rien n’échappe à l’enfant, notamment les silences de sa tante, une jeune femme qui aspire à une vie plus libre.</t>
+          <t>Namir et sa mère s’étaient jurés de refaire un film ensemble, mais la mort de Siham vient briser cette promesse. Pour tenir parole, Namir plonge dans l’histoire romanesque de sa famille. Cette enquête faite de souvenirs intimes et de grands films égyptiens se transforme en un récit de transmission joyeux et lumineux, prouvant que l’amour ne meurt jamais.</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Drame, Comédie</t>
+          <t>Documentaire</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>76</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>France, Egypt</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Wang Shang, Zhang Yanrong, Zhang Caixia, Cao Lingzhi, Zhou Haotian, Jiang Yien, Kaidong Yang</t>
+          <t>Siham Abdel Messeeh, Waguih Abdel Messeeh, Nermine Abdel Messeeh, Namir Abdel Messeeh</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Ours d'argent meilleure réalisation Berlin 2025, Berlinale 2025: Ours d'Argent de la Meilleure réalisation</t>
+          <t>Invité ADRC Cédric Lépine - Partenariat ADRC</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=2tyWSIt9SI8</t>
-        </is>
-      </c>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000018564.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000023001.html</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>["https://fr.web.img2.acsta.net/img/a2/ef/a2efaaf3096c8dfd6f96c92de831b657.jpg", "https://fr.web.img6.acsta.net/img/c9/f8/c9f8e54e38ef647d249b862e972f95d7.jpg", "https://fr.web.img3.acsta.net/img/1f/e4/1fe452cf587df5e34abc72efd9c946d8.jpg", "https://fr.web.img2.acsta.net/img/0d/00/0d00cb0edb801fc8f2c728b0b2f80a35.jpg", "https://fr.web.img2.acsta.net/img/10/46/10465bbb18492c1840b7f66cd73c19c4.jpg", "https://fr.web.img4.acsta.net/img/c6/86/c68641c59359989843921705dde08fb2.jpg", "https://fr.web.img5.acsta.net/img/a0/0d/a00dee7343ebfa281c8287f983a58349.jpg", "https://fr.web.img2.acsta.net/img/5e/d8/5ed83e10a02f07f59547e41d02786856.jpg", "https://fr.web.img2.acsta.net/img/c9/4d/c94d1e047516277c5979198d238ef48c.jpg", "https://fr.web.img2.acsta.net/img/0b/ce/0bce127a04b8ea212153c61ca62be1db.jpg", "https://fr.web.img5.acsta.net/img/8d/4b/8d4bc47451faafd3001e7ee1105093e0.jpg", "https://fr.web.img6.acsta.net/img/7a/28/7a288473ff1a7a8420dff10519510ba0.jpg", "https://fr.web.img2.acsta.net/img/11/8c/118c5519041b54a9dffb0a85758e90ef.jpg", "https://fr.web.img4.acsta.net/img/c1/d6/c1d67d545edf3ffa6397c13c9ea47eeb.jpg", "https://fr.web.img4.acsta.net/img/2c/c8/2cc8a012b929b6c60839ef5042789f22.jpg", "https://fr.web.img3.acsta.net/img/34/d7/34d7d4384752e727227f9b5561da6d59.jpg", "https://fr.web.img6.acsta.net/img/df/fd/dffd964e364f4101fb778d2805e09b7d.jpg", "https://fr.web.img5.acsta.net/img/09/9c/099cf115defcc05015c255be0366ebf3.jpg"]</t>
+          <t>["https://fr.web.img6.acsta.net/img/79/f6/79f6b79d81860c1d4cbb675e798e9c51.jpg", "https://fr.web.img6.acsta.net/img/11/d8/11d861d6f9d1a9a192534451c63aebfe.jpg", "https://fr.web.img6.acsta.net/img/20/2d/202d9475494d01d68afe9b192758fe6a.jpg", "https://fr.web.img4.acsta.net/img/20/e0/20e02fcbc855e9ac56c7e0e5b2af9083.jpg", "https://fr.web.img3.acsta.net/img/f2/55/f255c874fd57a8cd0695819635f5dfef.jpg", "https://fr.web.img5.acsta.net/img/6a/8b/6a8b3e37794df33406364b124212c25e.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Géniales</t>
+          <t>Baise-en-ville</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -659,164 +651,164 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Augusto Zanovello</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
+          <t>Martin Jauvat</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Invité ADRC Chloé Caye</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>SCOL</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>EauC 3 €</t>
-        </is>
-      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>https://fr.web.img5.acsta.net/c_310_420/img/ee/3b/ee3bfa8fa11ad1213889420794df5d24.jpg</t>
+          <t>https://fr.web.img6.acsta.net/c_310_420/img/8e/a5/8ea5ebba183c85d8c42b36a96b66d517.jpg</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Le programme GÉNIALES ! regroupe 4 courts métrages dans lesquels les héroïnes vont user de leur intelligence et créativité pour améliorer la vie de ceux ou celles qu’elles aiment. Des petites filles astucieuses dont la sagesse, la sagacité et l’ingéniosité leur permettront de relever des défis et d’accomplir de belles actions ! Quatre films qui donnent aux filles le pouvoir de changer les choses !Programme : - Lola et le piano à bruits d'Augusto Zanovello (2024 / France / Pologne / Suisse) : Lola est la grande sœur de Simon, 5 ans, qui vit dans son monde. En l'observant, elle remarque sa grande sensibilité aux petits sons cachés du quotidien. Avec son ami Rolih, Lola décide de construire une machine à bruits pour communiquer avec lui.- Entre deux sœurs d'Anne Sophie Gousset et Clément Céard (2022 / France) : Entre deux sœurs, il y a de la complicité et des rires. Entre deux sœurs, il y a l’amour comme moteur. Entre ces deux sœurs-là, il y a un petit quelque chose en plus, et c’est très bien comme ça.- Gonflées d'Alžbeta Mačáková Mišejková (2022 / République Tchèque) : Deux fillettes jouent tranquillement avec un ballon. Mais une querelle sans importance éclate au point de s’envoler, gonflées comme des ballons de baudruche ! Elles se retrouvent alors à flotter dans les airs sans pouvoir redescendre sur terre, au milieu d’autres duos en colère. Comment vont-elles se sortir de ce mauvais pas et sauver le chaton coincé sur un arbre ? ….- Princesse aubergine de Dina Velikovskaya (2023 / Allemagne) : Une reine et un roi ont tout ce qu’ils peuvent désirer, à part une chose… ils cherchent désespérément la graine qui leur permettra de voir naître un enfant pour égayer leur foyer. C’est alors qu’arrive dans le royaume une petite mendiante…</t>
+          <t>Quand sa mère menace de le virer du pavillon familial s’il ne se bouge pas les fesses, Sprite se retrouve coincé dans un paradoxe : il doit passer son permis pour trouver un taf, mais il a besoin d'un taf pour payer son permis. Heureusement, Marie-Charlotte, sa monitrice d'auto-école, est prête à tout pour l'aider - même à lui prêter son baise-en-ville. Mais... C'est quoi, au fait, un baise-en-ville ?</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Animation, Famille</t>
+          <t>Comédie</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr"/>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Zélie Chalvignac, Sacha Theotiste, Marie Schoenbock, Tom Guingand, Raphaël Scheer, Jennifer Tournaire, Morgane George, Sebastien Bizzotto</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr"/>
+          <t>Martin Jauvat, Emmanuelle Bercot, William Lebghil, Anaïde Rozam, Sébastien Chassagne, Annabelle Lengronne, Michel Hazanavicius, Jérôme Niel</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Invité ADRC Chloé Caye, Fondation Gan pour le cinéma 2024: Fondation Gan - Prix à la création</t>
+        </is>
+      </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>2025-02-12</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr"/>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=6CxCD9j5GBQ</t>
+        </is>
+      </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000004242.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000004512.html</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>["https://fr.web.img6.acsta.net/img/fb/ea/fbea0aaca8f9ca6af2b0aa957708921b.jpg", "https://fr.web.img6.acsta.net/img/bb/8b/bb8bf63655eb4520d44374839e18d570.jpg", "https://fr.web.img4.acsta.net/img/12/39/1239411f777d9b34ff99b45aa8ea1e5d.jpg", "https://fr.web.img2.acsta.net/img/69/13/69139306d0a39b28d04059998d782e17.jpg"]</t>
+          <t>["https://fr.web.img4.acsta.net/img/5f/fd/5ffdcbf01ced3064d847cf45f68f1e8c.jpg", "https://fr.web.img2.acsta.net/img/70/8d/708dafa0d7a642ba2daf451bddddf05f.jpg", "https://fr.web.img2.acsta.net/img/ae/2b/ae2b79db000bb6e752a33401378e5b4b.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Champions (Campeones)</t>
+          <t>La pire mère au monde</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>VO</t>
+          <t>VF</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Javier Fessier</t>
+          <t>Pierre Mazingarbe</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>SCOL</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Pass Culture 4 €</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Séance EPHAD HANDI</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>https://fr.web.img3.acsta.net/c_310_420/pictures/18/04/30/10/20/5882007.jpg</t>
+          <t>https://fr.web.img5.acsta.net/c_310_420/img/ea/fd/eafdfac8bc40d63ec84a32063363565a.jpg</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Marco occupe le prestigieux poste d’entraîneur-adjoint de l'équipe d'Espagne de basket. Mais son mauvais caractère lui pose problème. Après une série de déconvenues dont il est le seul responsable, Marco se retrouve à devoir coacher une équipe de déficients mentaux.</t>
+          <t>Louise de Pileggi, brillante substitut du procureur, a toujours eu des relations compliquées avec sa mère Judith qu’elle n’a pas vue depuis 15 ans. Quand elle se retrouve mutée au petit tribunal où Judith est greffière, Louise devient la cheffe de sa mère. Et pire encore : elles vont devoir collaborer dans une affaire à première vue banale, mais qui va mettre leurs nerfs à vif.</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Drame, Comédie</t>
+          <t>Comédie</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>119</t>
+          <t>85</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>France</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Javier Gutiérrez, Athenea Mata, Juan Margallo, José de Luna, Sergio Olmo, Jesús Vidal, Gloria Ramos, Alberto Nieto Fernández</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>Festival des rencontres cinématographique de Salon-de-Provence 2019: Prix des Lycéens, Goya 2019: Goya du meilleur film, Goya de la meilleure révélation masculine, Goya de la meilleure chanson</t>
-        </is>
-      </c>
+          <t>Louise Bourgoin, Muriel Robin, Florence Loiret Caille, Sébastien Chassagne, Gustave Kervern, Patrick Descamps, Anne Benoît, Johann Cuny</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr">
         <is>
-          <t>2018-06-06</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=uL3YLtGaGU4</t>
+          <t>https://www.youtube.com/watch?v=DubZRp9QwsI</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=256186.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=279638.html</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>["https://fr.web.img4.acsta.net/pictures/18/08/03/11/23/1783176.jpg", "https://fr.web.img3.acsta.net/pictures/18/04/30/09/41/0993026.jpg", "https://fr.web.img6.acsta.net/pictures/18/04/30/09/41/0977400.jpg", "https://fr.web.img6.acsta.net/pictures/18/04/30/09/41/0960213.jpg", "https://fr.web.img6.acsta.net/pictures/18/04/30/09/41/0941462.jpg", "https://fr.web.img3.acsta.net/pictures/18/04/30/09/41/0922712.jpg", "https://fr.web.img6.acsta.net/pictures/18/01/16/09/57/4351945.jpg"]</t>
+          <t>["https://fr.web.img4.acsta.net/img/fe/6a/fe6a2d1825f27579b5d5935d1662104f.jpg", "https://fr.web.img3.acsta.net/img/e3/d7/e3d7b58df0f285df881f289cb700433d.jpg", "https://fr.web.img2.acsta.net/img/4a/84/4a844cac98b2225c6a14af1700e6364b.jpg", "https://fr.web.img5.acsta.net/img/0b/e0/0be032fed7ca132697a0236a7442c00d.jpg", "https://fr.web.img2.acsta.net/img/0a/24/0a24e5bb15c4a635d0e3c405676d89b9.jpg", "https://fr.web.img3.acsta.net/img/44/40/444070ee5a8b27c077b983c32e328e95.jpg", "https://fr.web.img6.acsta.net/img/ee/14/ee1484bc856187e7bf54eb4fbc174baf.jpg", "https://fr.web.img5.acsta.net/img/c5/bf/c5bfdaba870ea3b8d87591a083f65456.jpg", "https://fr.web.img6.acsta.net/img/84/69/846975d92773ae0155e3482afb5b4b7f.jpg", "https://fr.web.img2.acsta.net/img/f7/a5/f7a5493041d5a798c783b71a27d026d5.jpg", "https://fr.web.img6.acsta.net/img/5d/b2/5db2f573ff0656b97aff4e839aa30813.jpg", "https://fr.web.img2.acsta.net/img/55/c3/55c32fa89f9070f778c0b90141ff9a1d.jpg", "https://fr.web.img2.acsta.net/img/f0/af/f0af70e4e07ef7f8732123cf6129a461.jpg", "https://fr.web.img5.acsta.net/img/c4/52/c45239fce1251f2373fdec9facf110e0.jpg", "https://fr.web.img4.acsta.net/img/c4/d6/c4d6d97e38ef1575d1183be1e33620bf.jpg", "https://fr.web.img2.acsta.net/img/c5/6c/c56c7f470fc89e634f8c8b8c04da0510.jpg", "https://fr.web.img5.acsta.net/img/b4/13/b4133a66dc6e338546c3df28d75ccf78.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -826,84 +818,80 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Los tigres</t>
+          <t>Victor comme tout le monde</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>VO</t>
+          <t>VF</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Alberto Rodriguez</t>
-        </is>
-      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Coup de cœur</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>https://fr.web.img3.acsta.net/c_310_420/img/e6/07/e6072a30a6045a3cdc545da6bbafe62a.jpg</t>
+          <t>https://fr.web.img3.acsta.net/c_310_420/img/17/7a/177a42854bab65ac4e585d4064bc3bee.jpg</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Frère et sœur, Antonio et Estrella travaillent depuis toujours comme scaphandriers dans un port espagnol sur les navires marchands de passage. En découvrant une cargaison de drogue dissimulée sous un cargo qui stationne au port toutes les trois semaines, Antonio pense avoir trouvé la solution pour résoudre ses soucis financiers : voler une partie de la marchandise et la revendre.</t>
+          <t>Habité par Victor Hugo, le comédien Robert Zucchini traîne une douce mélancolie lorsqu'il n'est pas sur scène. Chaque soir, il remplit les salles en transmettant son amour des mots. Jusqu’au jour où réapparaît sa fille, qu’il n’a pas vue grandir… Et si aimer, pour une fois, valait mieux qu’admirer ?</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Policier</t>
+          <t>Comédie dramatique</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>88</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Spain, France</t>
+          <t>France</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Antonio de la Torre, Bárbara Lennie, Joaquín Núñez, César Vicente, Skone, Jesús del Moral, Silvia Acosta</t>
+          <t>Fabrice Luchini, Chiara Mastroianni, Louise Orry-Diquéro, Suzanne De Baecque, Marie Narbonne, Lauretta Trefeu, Iris Bry, Naidra Ayadi</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-03-11</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=jza6K4qC6s8</t>
+          <t>https://www.youtube.com/watch?v=t0RrVuOml0M</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=325967.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000021956.html</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>["https://fr.web.img2.acsta.net/img/37/94/37949144d663b9ea2b4260cf3b852cd9.jpg", "https://fr.web.img5.acsta.net/img/9c/75/9c75f82261a778386435eb4212f11dd7.jpg", "https://fr.web.img6.acsta.net/img/15/b0/15b0091883c4b700c404c6d0382b49f4.jpg", "https://fr.web.img3.acsta.net/img/e7/ca/e7ca5d2af12192044bd09a671482a6b6.jpg", "https://fr.web.img6.acsta.net/img/34/47/3447f48c4438cc923df9e2a3a8e98fa2.jpg"]</t>
+          <t>["https://fr.web.img4.acsta.net/img/e9/87/e987439316c89fa9fecbc48c10843d0a.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -913,98 +901,98 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>La petite cuisine de Mehdi</t>
+          <t>Le grand Phuket</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Amine Adjina</t>
+          <t>Liu Yaonan</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Séance EPHAD HANDI - Famille</t>
-        </is>
-      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Ciné Jeunes du samedi 18h</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
-          <t>TU 5 €</t>
+          <t>Avant-Première en Compétition</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>https://fr.web.img2.acsta.net/c_310_420/img/b1/f3/b1f3ff9d44ec565d42e1b1ac5cd2a170.jpg</t>
+          <t>https://fr.web.img6.acsta.net/c_310_420/img/c9/8a/c98a620996904fb707ac74e2ee152db7.jpg</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Mehdi est sur un fil. Il joue le rôle du fils algérien parfait devant sa mère Fatima, tout en lui cachant sa relation avec Léa ainsi que sa passion pour la gastronomie française. Il est chef dans un bistrot qu’il s’apprête à racheter avec Léa. Mais celle-ci n’en peut plus de ses cachoteries et exige de rencontrer Fatima. Au pied du mur, Mehdi va trouver la pire des solutions.</t>
+          <t>Li Xing, 14 ans, vit dans le sud de la Chine, dans le district de Great Phuket, en pleine reconstruction. Il s'entend mal avec sa mère, qui refuse de quitter la maison familiale vouée à la destruction. Le collège où il étudie ne lui apporte que des ennuis. Un jour, il trouve un refuge souterrain où il peut échapper à sa vie d'adolescent et où d'étranges événements se produisent…</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Comédie</t>
+          <t>Drame, Mystère</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>98</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Belgium, Germany, France, Hong Kong</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Younès Boucif, Clara Bretheau, Hiam Abbass, Gustave Kervern, Laurent Stocker, Lou-Adriana Bouziouane, Malika Zerrouki, Birane Ba</t>
+          <t>Li Rongkun, Yang Xuan, You Junwen, Liu Huiyun, Kang Hang, Xie Zhenan, Liu Lijun, Yan Huimei</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=E0ca-rNdx-k</t>
+          <t>https://www.youtube.com/watch?v=8gZJSKZs-to</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000012569.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=326632.html</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>["https://fr.web.img3.acsta.net/img/56/5d/565d45495a749aa8590be50bdb7e6a52.png", "https://fr.web.img4.acsta.net/img/80/43/804364ed53ae314c9c8f4dbb629a4db5.jpg", "https://fr.web.img6.acsta.net/img/3c/43/3c431fa9f9a9c36aaafc380bb67cf313.jpg", "https://fr.web.img3.acsta.net/img/c8/b5/c8b568005bff539cccf9fd010e33e0dc.jpg", "https://fr.web.img5.acsta.net/img/a2/32/a2323e1400ca48d2ba5d6af799c6def9.jpg", "https://fr.web.img4.acsta.net/img/3d/eb/3deb4a2b5708fde4d12caa4d0642fb92.jpg", "https://fr.web.img6.acsta.net/img/c7/45/c745fd872d79b6df40df37ced783fdd1.jpg", "https://fr.web.img6.acsta.net/img/83/8d/838d299f3116d20809b3a5a396cef2af.jpg"]</t>
+          <t>["https://fr.web.img3.acsta.net/pictures/24/02/12/09/34/1081778.jpg", "https://fr.web.img6.acsta.net/pictures/24/02/12/09/34/1063058.jpg", "https://fr.web.img6.acsta.net/pictures/24/02/12/09/34/1049018.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Le pays d'Arto</t>
+          <t>En route</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1015,79 +1003,71 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Tamara Stepanyan</t>
+          <t>Alexei Mironov</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Ciné goûter JP</t>
+        </is>
+      </c>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Avant-Première</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>https://fr.web.img6.acsta.net/c_310_420/img/f7/38/f738c353019cfe13d0d338999dd2cc4b.jpg</t>
+          <t>https://fr.web.img5.acsta.net/c_310_420/img/35/69/3569e5f8d0bdaf83fc6eed80f9372f9a.jpg</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Céline arrive pour la première fois en Arménie afin de régulariser la mort d’Arto, son mari. Elle découvre qu’il lui a menti, qu’il a fait la guerre, usurpé son identité, et que ses anciens amis le tiennent pour un déserteur. Commence pour elle un nouveau voyage, à la rencontre du passé d'Arto : invalides des combats de 2020, vétérans de guerre, hantises d’une guerre qui n’en finit jamais. Une femme court après un fantôme. Comment faire pour l’enterrer ? Peut-on sauver les morts ?</t>
+          <t>Qu’il est bon de parcourir le monde ou simplement découvrir son environnement… Ici ou là, nos petits aventuriers : une charmante escargote, une fratrie de lapereaux, un jeune dragon, deux sœurs hermines, un agneau dans les nuages, et un petit garçon vont cheminer, naviguer, explorer et s’entraider. Chaque jour est un nouveau chemin pour grandir, s’émerveiller et s’ouvrir au monde.Programme :- L’Escargote à Paris d'Alexei Mironov et Yulia Matrosova (Russie, 4', 2014) : C’est parti pour notre petite escargote qui décide d’aller faire le tour du Monde. Au détour de son voyage qui l’amène à Londres, à Moscou et au Mexique, elle se pose à Paris. Rien de plus enrichissant que de découvrir d’autres cultures, et, au gré des rencontres, de s’enrichir de ce que les autres peuvent nous apporter. Mais qu’il est bon aussi de rentrer chez soi et de s’apercevoir que les vrais amis, sont ceux que nous choisissons avec le cœur.- Sevanik, le petit dragon de Harutyun Tumaghyan (Arménie, 7', 2023) : Sevanik est un petit dragon vivant dans le lac Sevan. Il n’a qu’un seul ami : un nuage duveteux. Ce nuage, un peu comme un parent ou un ange, suit chacun de ses mouvements et de ses émotions. Mais un jour, Sevanik décide de s’aventurer en dehors du lac pour découvrir la Terre ferme. Il se fait piquer par un moustique. Cet incident va chambouler les deux amis, les obliger à changer leurs habitudes et modifier leur regard sur les autres.- La Balade de Mazayka de Yuri Chaika-Pronin (Russie, 4', 2023) : Le légendaire grand-père Mazaito s’est donné pour mission de sauver de la noyade tous les animaux pris par les eaux. Chantant à la barre de sa barque, il récupère lapins et loups pour leur offrir un asile sûr sur la terre ferme.- Mû et la source divine de Malin Neumann (Allemagne, 6', 2024) : Suite à une sécheresse extrême, la source divine s’est tarie et Mû décide de partir à la recherche d’eau, indispensable pour la relancer. Accompagné de son animal de compagnie, il entreprend alors un voyage jusqu’au bout du monde et jusqu’au plus haut sommet. Mais, malgré ses efforts, sa tentative échoue. Du moins le croit-il car, finalement, un évènement inattendu va redonner vie à la source.- Aller &amp; retour de Lucia Bulgheroni et Michele Greco (Italie, 9', 2025) : Aller et Retour sont deux hermines qui à l’arrivée de l’hiver vont devoir chercher de la nourriture pour survivre. Si jeune et si vulnérable, elles vont devoir faire face à un grand danger. Que se passera-t-il quand Aller sera kidnappée ? Retour devra alors se mettre en route pour sauver sa sœur.- Songe d'un petit agneau de Hamid Karimian (Iran, 5', 2015) : Un jeune agneau s’est égaré dans une forêt inquiétante. Seul et perdu, la peur le gagne… quand soudain il perçoit les douces notes de la flûte d’un berger ! Envoûté par la volupté de la musique, l’agneau se laisse alors emporter dans un voyage imaginaire et féerique dans lequel ses craintes n’ont plus de place et qui le ramène au sein de son troupeau.</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Drame</t>
+          <t>Animation, Famille</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>104</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>France, Armenia</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>Camille Cottin, Zar Amir Ebrahimi, Shant Hovhannisyan, Hovnatan Avédikian, Ալեքսանդր Խաչատրյան, Babken Chobanyan, Denis Lavant, Hasmik Suvaryan</t>
-        </is>
-      </c>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>https://vimeo.com/1145317304</t>
-        </is>
-      </c>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=325261.html</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>["https://fr.web.img6.acsta.net/img/8e/91/8e91480981bb0b222065082f48fd1bf8.jpg", "https://fr.web.img2.acsta.net/img/9c/26/9c260bd73b97baf501804471498d3c7d.jpg"]</t>
-        </is>
-      </c>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000031073.html</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Imago</t>
+          <t>Urchin</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1098,442 +1078,510 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Déni Oumar Pitsaev</t>
+          <t>Harris Dickinson</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition</t>
+        </is>
+      </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>https://fr.web.img4.acsta.net/c_310_420/img/da/44/da449a072ddfc0a919bbc108612c9bf2.jpg</t>
+          <t>https://fr.web.img6.acsta.net/c_310_420/img/e7/82/e782432beca8a04cea3b2dc66459c4a5.jpg</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Déni est le nouveau propriétaire d’un petit lopin de terre dans une vallée isolée en Géorgie, à la frontière de la Tchétchénie dont il est exilé depuis l’enfance. Il débarque là-bas et projette d’y construire une maison qui tranche drôlement avec les coutumes locales. Un fantasme qui ravive ses souvenirs et ceux de son clan déraciné qui pourtant ne rêve que d'une chose, le marier !</t>
+          <t>À Londres, Mike vit dans la rue, il va de petits boulots en larcins, jusqu'au jour où il se fait incarcérer. À sa sortie de prison, aidé par les services sociaux, il tente de reprendre sa vie en main en combattant ses vieux démons.</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Documentaire, Drame</t>
+          <t>Drame, Comédie</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>99</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>France, Belgium, Georgia</t>
+          <t>United Kingdom, United States of America</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Déni Oumar Pitsaev</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr"/>
+          <t>Frank Dillane, Megan Northam, Карина Химчук, Shonagh Marie, Amr Waked, Claudia Jones, Shahzad Ali, Michael Quartey</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Festival de Cannes 2025: Un Certain Regard - Prix du meilleur acteur</t>
+        </is>
+      </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=gv-r5m2WtNs</t>
+          <t>https://www.youtube.com/watch?v=4cJL6vmYOeo</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=317102.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000019912.html</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>["https://fr.web.img5.acsta.net/img/f6/8e/f68e3fea8b975fe0a57e4b0f36535713.jpg", "https://fr.web.img6.acsta.net/img/9e/f1/9ef1bee9b89474879ca8fd3c462bc402.jpg", "https://fr.web.img5.acsta.net/img/eb/9f/eb9f0854701ddd165e7f31080d959b8d.jpg", "https://fr.web.img3.acsta.net/img/ca/5a/ca5ae1439ccab66efa2a95a349f76c5b.jpg", "https://fr.web.img3.acsta.net/img/e4/81/e481242c0f8602779063a887414e6a0d.jpg"]</t>
+          <t>["https://fr.web.img5.acsta.net/img/bb/78/bb784f39d4843f599afba87529b2c028.jpg", "https://fr.web.img2.acsta.net/img/df/3d/df3dc86c2a96673a0d49796581ea5929.jpg", "https://fr.web.img4.acsta.net/img/1e/44/1e4451e35e6059ee33003bb1ddbe8b9c.jpg", "https://fr.web.img2.acsta.net/img/2d/a2/2da21da8e6c084f763290e30f0e31548.jpg", "https://fr.web.img6.acsta.net/img/da/30/da301edeec034ee0839592ee70672741.jpg", "https://fr.web.img4.acsta.net/img/fc/1e/fc1e3b1ba4bbd2e5fb722ed5f0b294e3.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>21:15</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Elles inspirent</t>
+          <t>Noise</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Lila Carlier</t>
+          <t>Soo-jin Kim</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Rencontre Lila Carlier réalisatrice, et partenariat avec Nous Vous Elles</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>https://fr.web.img6.acsta.net/img/14/b1/14b1a952a540a054f5ffe0712e82ab86.jpg</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Ju-young, malentendante, découvre que sa sœur a mystérieusement disparu de son appartement. En cherchant des réponses, elle se heurte à des voisins terrifiés, obsédés par le silence, et à une atmosphère de plus en plus oppressante. La nuit, des bruits inexpliqués résonnent dans l’immeuble déserté, éveillant une présence invisible. Ce qu’elle croyait être une simple disparition devient une plongée terrifiante dans un cauchemar hanté par le silence.</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Epouvante-horreur, Thriller</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>2023-04-14</t>
+        </is>
+      </c>
       <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=325653.html</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>["https://fr.web.img6.acsta.net/img/16/2e/162eb2cb9a4301b8b93a8ce08ba24416.jpg"]</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Stups</t>
+          <t>Les fleurs du manguier</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Alice Odiot, Jean-Robert Viallet</t>
+          <t>Akio Fujimoto</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Partenariat avec Empreinte Carbonne</t>
-        </is>
-      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition</t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>https://fr.web.img2.acsta.net/c_310_420/img/77/e7/77e79153a041d19463f7b4cd81b3629c.jpg</t>
+          <t>https://fr.web.img6.acsta.net/img/b4/c1/b4c1790cacbd833589c6a4de26805535.jpg</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Une grande porte en métal qui coulisse pour laisser entrer les fourgons de la Police. Des hommes en sortent, avec leurs histoires. Des murs, des geôles, des escaliers en pierre, des salles d’audience, des coulisses, des larmes, des cris, des regards. Le tribunal de Marseille est débordé par les affaires de stupéfiants. Ceux qui sont jugés là sont les gérants d’une économie du chaos. Ce sont aussi les petits travailleurs du shit, des enfants qui ont grandi seuls. En contrebas, le port, au loin, les quartiers périphériques, la ville bouillante, remplie de ses blessures. De ses beautés aussi.</t>
+          <t>Dans l'espoir de retrouver leur famille dispersée, Shafi, 4 ans, et sa sœur Somira, 9 ans, quittent un camp Rohingyas du Bangladesh pour rejoindre la Malaisie. Guidés par leur regard d’enfant, ils entreprennent une traversée périlleuse.</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Documentaire</t>
+          <t>Drame</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>99</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>France</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
+          <t>Japan, France, Malaysia, Germany</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Muhammad Shofik Rias Uddin, Shomira Rias Uddin</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Mostra de Venise 2025: Prix spécial du jury Orizzonti</t>
+        </is>
+      </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-08-31</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=OGuqIZZzmo4</t>
+          <t>https://www.youtube.com/watch?v=ZNyi9LzJkb4</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000025677.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000027824.html</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>["https://fr.web.img6.acsta.net/img/c2/79/c279d7ffe0bdde3e3dac1276ebeb9ebc.jpg", "https://fr.web.img3.acsta.net/img/58/62/58629d8b62c061e2fc7ca42379f842c4.jpg", "https://fr.web.img4.acsta.net/img/6d/31/6d31c13aba66eb38021880767046af9e.jpg", "https://fr.web.img2.acsta.net/img/8f/39/8f3982abf3ca906110fc4e5dfe79745b.jpg", "https://fr.web.img3.acsta.net/img/48/ef/48ef4963e3919d04ff5ffa1a16227678.jpg", "https://fr.web.img6.acsta.net/img/7b/e2/7be26a46c96f06bf490cbfe0c93090e9.jpg", "https://fr.web.img6.acsta.net/img/36/93/3693a5b82d83cb2683c8640a2f1b466e.jpg", "https://fr.web.img6.acsta.net/img/9b/11/9b111376eaf9777d335ffbbfb7110816.jpg"]</t>
+          <t>["https://fr.web.img4.acsta.net/img/a0/ce/a0ce92b38c457f2b9817375347c75c80.jpg", "https://fr.web.img2.acsta.net/img/3c/5a/3c5af433d706b834e7dc8a8182960a5a.jpg", "https://fr.web.img6.acsta.net/img/00/fb/00fbc4831a05563c3d66fe690b5a9d5f.jpg", "https://fr.web.img5.acsta.net/img/31/97/3197ea34f7123218da9f5b62b0233282.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Les cavaliers des terres sauvages</t>
+          <t>Sauvage</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>VO</t>
+          <t>VF</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Mickaël Dweck, Gregory Kershaw</t>
+          <t>Camille Ponsin</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition</t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>https://fr.web.img6.acsta.net/c_310_420/img/07/0b/070bd200f493a4edb86ef38eb8b529a5.jpg</t>
+          <t>https://fr.web.img6.acsta.net/img/18/1a/181a47be9ff7a00987d7387430b36139.jpg</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Au cœur des montagnes argentines, vit une petite communauté de gauchos, des familles de cavaliers profondément attachées à la nature et perpétuant leurs traditions. Tandis que les anciennes générations partagent leur sagesse, leurs rites et culture, leur descendance tente de préserver leur identité dans un monde en pleine mutation.</t>
+          <t>Au cœur d’une vallée reculée des Cévennes, des néo-ruraux vivent en autarcie, ne s’interdisant rien et partageant tout. Chacun y trouve sa place, son compte, son but. Chacun, sauf Anja. Enfant insaisissable et perturbée, elle va un jour fuir pour aller vivre à l’état quasi sauvage dans les bois alentour mettant à mal le fragile équilibre de la communauté. Inspiré d’une histoire vraie.</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Documentaire</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>84</t>
-        </is>
-      </c>
+          <t>Drame</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Argentina, Greece, United States of America</t>
+          <t>France</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Guada Gonza, Tati Gonza, Jony Avalos, Solano Avalos</t>
+          <t>Lou Lampros, Céline Sallette, Bertrand Belin</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=dBcjVDZL6Kc</t>
-        </is>
-      </c>
+          <t>2026-04-08</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=325059.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000007389.html</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>["https://fr.web.img5.acsta.net/img/93/9a/939afdfe90ce0386c81b8d139cd0165a.jpg", "https://fr.web.img4.acsta.net/img/45/33/45333442ea8efd717096562f327ebd3d.jpg", "https://fr.web.img5.acsta.net/img/60/f7/60f79148624dc7bccb5729f31bdd9eb9.jpg", "https://fr.web.img5.acsta.net/img/74/2e/742e5618400c291f2cb1fd32ed5671a7.jpg", "https://fr.web.img6.acsta.net/img/97/9c/979cbb972d2cce4fbdc9e4f6dd29dbf8.jpg", "https://fr.web.img6.acsta.net/img/7c/8a/7c8ab3088aaaf0112ef2f7840a34b1f8.jpg", "https://fr.web.img5.acsta.net/img/7a/ed/7aedee13fafebdca46ef845a4d07ec80.jpg"]</t>
+          <t>["https://fr.web.img4.acsta.net/img/92/bf/92bf0fb31086774f583f545151103a6c.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Tout est parti d'ici</t>
+          <t>I swear</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Vincent Barthe</t>
+          <t>Kirk Jones</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>rencontre Vincent Barthe, réalisateur</t>
-        </is>
-      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition</t>
+        </is>
+      </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>https://fr.web.img2.acsta.net/img/54/91/5491512e91d6c2483f4a4eafb579c81b.jpg</t>
+          <t>https://fr.web.img5.acsta.net/c_310_420/img/1c/f8/1cf8c5c5caa2a19a90d78914da6416f7.jpg</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>En 1939, la découverte d’un gisement d’hydrocarbures à Saint-Marcet, dans le Comminges, réveille l’espoir d’un développement local et d’une puissance industrielle nationale. De cette campagne tranquille naît une aventure qui donnera lieu à la création de la Régie Autonome des Pétroles (RAP), ancêtre d’ELF, qui deviendra l’un des plus grands groupes industriels français. Les foreurs commingeois partent conquérir les gisements d’Algérie, et font le prospérité d’un groupe industriel public. La mémoire locale s’efface. Aujourd’hui, les traces sont ténues, presque invisibles, et les récits fragmentaires. Par une démarche documentaire minutieuse et participative, ce film ravive une mémoire industrielle oubliée et redonne une place aux voix locales. Une plongée dans un XXe siècle fait d’espoirs, de conquêtes, de renoncements et de silence.</t>
+          <t>L'histoire vraie et le parcours semé d'embûches de John Davidson, un adolescent atteint du syndrome de la Tourette, une maladie encore méconnue dans les années 1980.</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>Drame</t>
+          <t>Drame, Biopic</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
+          <t>121</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>United Kingdom, Ireland</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Robert Aramayo, Maxine Peake, Shirley Henderson, Peter Mullan, Scott Ellis Watson, Sanjeev Kohli, Ron Donachie, Steven Cree</t>
+        </is>
+      </c>
       <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>2026-04-08</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=oeWqQN3snCU</t>
+        </is>
+      </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000030494.html</t>
-        </is>
-      </c>
-      <c r="U12" t="inlineStr"/>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000009982.html</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>["https://fr.web.img6.acsta.net/img/98/9e/989ef532221684aa7746216d15267395.jpg", "https://fr.web.img6.acsta.net/img/70/18/70189dfd2025cfd793467526b00a214e.jpg", "https://fr.web.img6.acsta.net/img/bb/28/bb28d97eb5f9d7a6490a67cbb11dcab2.jpg", "https://fr.web.img4.acsta.net/img/97/38/9738737f981755f47fac4ae5e014beb8.jpg", "https://fr.web.img2.acsta.net/img/d9/40/d9407b614190b30e0626fbd1049eae33.jpg", "https://fr.web.img3.acsta.net/img/6b/e4/6be422c2ab0c37d8d576163727d27639.jpg", "https://fr.web.img2.acsta.net/img/32/49/32494080ea26a9ab5cf160990bd16f2b.jpg", "https://fr.web.img3.acsta.net/img/ae/86/ae86246f761f58aa29eeff665daef98d.jpg", "https://fr.web.img6.acsta.net/img/7b/ff/7bff646f1cfe461e1fbe2fa0f9a5dab2.jpg", "https://fr.web.img2.acsta.net/img/8b/f7/8bf78a61a305680944e06c8e34f3a294.jpg", "https://fr.web.img6.acsta.net/img/c4/92/c49243ebe789ea388e4781f4d701c9c5.jpg", "https://fr.web.img3.acsta.net/img/24/f8/24f8601263c3732cc5c947b5472d28cc.jpg", "https://fr.web.img4.acsta.net/img/24/ef/24efce29c062578347603c1115087363.jpg", "https://fr.web.img5.acsta.net/img/01/8c/018c61a8473809bf69ffb453092d813e.jpg", "https://fr.web.img2.acsta.net/img/b3/f3/b3f32b141ab8950d111a60451cccf3dd.jpg", "https://fr.web.img6.acsta.net/img/5b/8a/5b8a3daf65b91b6f7f9f323823b25f1e.jpg", "https://fr.web.img4.acsta.net/img/f9/77/f977a3d6fffcb3d149350eecfacf3dba.jpg", "https://fr.web.img6.acsta.net/img/ff/08/ff08181aaf0e101ff247f5ee4620df45.jpg", "https://fr.web.img2.acsta.net/img/de/fb/defb2b502a2f7a0ba41042967ebfc92f.jpg"]</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>17:15</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Pompei, sotto le nuvole</t>
+          <t>Ma frère</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>VO</t>
+          <t>VF</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Gianfranco Rosi</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
+          <t>Lise Akoka, Romane Gueret</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Prix du jury et Prix du jury presse Pauillac 2025</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
-          <t>https://fr.web.img6.acsta.net/c_310_420/img/7c/9b/7c9b1938b3f8723050ce45f800993b21.jpg</t>
+          <t>https://fr.web.img5.acsta.net/c_310_420/img/35/23/35233aa3767ab31d242ec1c3ff34497c.jpg</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Pompéi, Naples, le Vésuve. Des vies sous la menace du volcan : archéologues, pompiers, éducateurs, marins, photographes… La terre tremble et le passé infuse dans le présent de tous. En donnant voix aux habitants, le film compose un portrait inédit de la ville, comme une machine à voyager dans le temps.</t>
+          <t>Shaï et Djeneba ont 20 ans et sont amies depuis l’enfance. Cet été-là, elles sont animatrices dans une colonie de vacances. Elles accompagnent dans la Drôme une bande d’enfants qui, comme elles, ont grandi entre les tours de la Place des Fêtes à Paris. À l’aube de l’âge adulte, elles devront faire des choix pour dessiner leur avenir et réinventer leur amitié.</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Documentaire</t>
+          <t>Comédie</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>112</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Italy, France</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr"/>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Fanta Kebe, Shirel Nataf, Zakaria-Tayeb Lazab, Mouctar Diawara, Idir Azougli, Yuming Hey, Suzanne De Baecque, Amel Bent</t>
+        </is>
+      </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Mostra de Venise 2025: Prix Spécial du Jury</t>
+          <t>Prix du jury et Prix du jury presse Pauillac 2025</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>2025-11-19</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=eF_RPx6CXFw</t>
+          <t>https://www.youtube.com/watch?v=53BgM9euEOQ</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000022228.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000007387.html</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>["https://fr.web.img6.acsta.net/img/c9/0c/c90cebd070bd9bd29fa4567f2be3e28e.jpg"]</t>
+          <t>["https://fr.web.img3.acsta.net/img/98/b8/98b83a6cafcd5ae0c8a89c20f9ae7437.jpg", "https://fr.web.img2.acsta.net/img/37/9d/379dbf504a6aee9a25b25e1c699b25c3.jpg", "https://fr.web.img4.acsta.net/img/5e/08/5e08b0482694b6ce002742071afe0b45.jpg", "https://fr.web.img6.acsta.net/img/2d/c0/2dc0c49d0be726b94b67121cac743537.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>L'agent secret</t>
+          <t>Tatouage</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1544,81 +1592,77 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Kleber Mendonça Filho</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Prix mise en scène et interprétation masculine Cannes 2025</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Coup de coeur</t>
-        </is>
-      </c>
+          <t>Yasuzo Masumura</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Soirée avec Pup En Vol + invité (à préciser) - Partenariat ADRC</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
-          <t>https://fr.web.img5.acsta.net/c_310_420/img/d5/da/d5dae089c320b75bf1903cc249165073.jpg</t>
+          <t>https://fr.web.img6.acsta.net/c_310_420/img/d1/e0/d1e0f786717651d20890faeb1892977b.jpg</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Brésil, 1977. Marcelo, un homme d’une quarantaine d’années fuyant un passé trouble, arrive dans la ville de Recife où le carnaval bat son plein. Il vient retrouver son jeune fils et espère y construire une nouvelle vie. C’est sans compter sur les menaces de mort qui rôdent et planent au-dessus de sa tête…</t>
+          <t>La jeune Otsuya et son amant Shinsuke fuient la maison familiale pour vivre leur amour et trouvent refuge chez Gonji, un escroc qui se prétend être leur ami mais il les trahit. Il vend la jeune fille au tenancier d’une maison de geishas qui fait tatouer sur le dos d’Otsuya une araignée à tête humaine dans le but de briser sa volonté. Le contraire se produit et le tatouage métamorphose Otsuya. Elle devient une geisha sans scrupule et extermine les hommes qui ont fait son malheur. Manipulatrice et sanguinaire, elle semble possédée par l’araignée gravée sur sa peau…</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Policier, Drame</t>
+          <t>Drame</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>86</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Brazil, France, Germany, Netherlands, Argentina</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Wagner Moura, Carlos Francisco, Tânia Maria, Robério Diógenes, Roney Villela, Gabriel Leone, Alice Carvalho, Hermila Guedes</t>
+          <t>Ayako Wakao, 長谷川明男, 山本學, 佐藤慶, 須賀不二男, Asao Uchida, 藤原礼子, 毛利菊枝</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Festival de Cannes 2025: Prix de la mise en scène, Prix d'interprétation masculine</t>
+          <t>Soirée avec Pup En Vol + invité (à préciser) - Partenariat ADRC</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2004-12-22</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=8-9Sa_vHlZg</t>
+          <t>https://www.youtube.com/watch?v=gb9DKq21rDA</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000009761.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=25663.html</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>["https://fr.web.img3.acsta.net/img/55/23/552378c49a9cdcf3821395a4ca142079.jpg", "https://fr.web.img6.acsta.net/img/c1/c5/c1c563573e879fe9ee0a00355a136b3d.jpg", "https://fr.web.img5.acsta.net/img/02/4c/024cc7daa15d58e40a29c4aa0ef452be.jpg"]</t>
+          <t>["https://fr.web.img3.acsta.net/pictures/22/10/03/11/59/2217050.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1628,94 +1672,79 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Lady Nazca</t>
+          <t>A pied d'œuvre</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>VO</t>
+          <t>VF</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Damien Dorsaz</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr"/>
+          <t>Valérie Donzelli</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Partenariat ADRC</t>
+        </is>
+      </c>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Découverte</t>
-        </is>
-      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>https://fr.web.img5.acsta.net/c_310_420/img/ff/55/ff55502555d7b33a61e0af53fd5dda56.jpg</t>
-        </is>
-      </c>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Pérou, 1936. Maria, jeune enseignante à Lima, rencontre Paul d’Harcourt, archéologue français. Ce dernier l’emmène dans le désert de Nazca où elle découvre un vestige millénaire qui va peu à peu devenir le combat de sa vie… D’après une histoire vraie. Inspiré de la vie de l'archéologue Maria Reiche.</t>
+          <t>Achever un texte ne veut pas dire être publié, être publié ne veut pas dire être lu, être lu ne veut pas dire être aimé, être aimé ne veut pas dire avoir du succès, avoir du succès n'augure aucune fortune.
+ À Pied d’œuvre raconte l'histoire vraie d'un photographe à succès qui abandonne tout pour se consacrer à l'écriture, et découvre la pauvreté.</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>Biopic, Aventure, Drame, Historique</t>
+          <t>Comédie, Drame</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>92</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Germany, France, Switzerland</t>
+          <t>France</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Devrim Lingnau, Guillaume Gallienne, Olivia Ross, Amaranta Kun, Jorge Pomacanchari, Víctor Prada</t>
+          <t>Bastien Bouillon, Marie Rivière, Virginie Ledoyen, André Marcon, Pauline Clément, Arthur Dupont, Émilie Caen, Quentin Dolmaire</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
-        </is>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=tWJgRr7PQs0</t>
-        </is>
-      </c>
-      <c r="T15" t="inlineStr">
-        <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=295609.html</t>
-        </is>
-      </c>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>["https://fr.web.img4.acsta.net/img/6f/5e/6f5efc14604010b9991442991f535ba7.jpg", "https://fr.web.img5.acsta.net/img/bc/a7/bca73712eac7e8cd008c05778564e0c4.jpg", "https://fr.web.img2.acsta.net/img/f8/84/f8842e5ab912daf3f4de67b5ac47d59b.jpg", "https://fr.web.img4.acsta.net/img/14/f2/14f2871c8e4c521588b7b90a3c02ae5e.jpg", "https://fr.web.img2.acsta.net/img/96/5a/965a3f620b6953ebf0b27678b3b42e02.jpg"]</t>
-        </is>
-      </c>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Furcy, né libre</t>
+          <t>Alter ego</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1726,37 +1755,29 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Abd Al Malik</t>
+          <t>Nicolas Charlet, Bruno Lavaine</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>Découverte</t>
-        </is>
-      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
-          <t>https://fr.web.img6.acsta.net/c_310_420/img/51/04/5104c913367b4e8dc4d89d55c7c965ae.jpg</t>
+          <t>https://fr.web.img6.acsta.net/img/8e/e1/8ee1e2ac450dea02a69bf8cabb0b74a6.jpg</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Île de la Réunion, 1817. À la mort de sa mère, l'esclave Furcy découvre des documents qui pourraient faire de lui un homme libre. Avec l’aide d’un procureur abolitionniste, il se lance dans une bataille judiciaire pour la reconnaissance de ses droits. Inspiré d’une histoire vraie. Adaptée du livre "L'Affaire de l'esclave Furcy" de Mohammed Aïssaoui.</t>
+          <t>Alex a un problème : son nouveau voisin est son sosie parfait. Avec des cheveux. Un double en mieux, qui va totalement bouleverser son existence.</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>Historique, Drame, Judiciaire, Biopic</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>108</t>
-        </is>
-      </c>
+          <t>Comédie</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr">
         <is>
           <t>France</t>
@@ -1764,128 +1785,132 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Makita Samba, Romain Duris, Ana Girardot, Vincent Macaigne, Liya Kebede, Frédéric Pierrot, André Marcon, Micha Lescot</t>
+          <t>Laurent Lafitte, Olga Kurylenko, Blanche Gardin, Valérie Donzelli, Monsieur Fraize, Zabou Breitman, Bertrand Goncalves</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
-        </is>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=cPzOCjo8wos</t>
-        </is>
-      </c>
+          <t>2026-01-23</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=292718.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=288260.html</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>["https://fr.web.img4.acsta.net/img/6f/48/6f488e969255f17b9ec47ab60024564d.jpg", "https://fr.web.img6.acsta.net/img/8d/73/8d73ef2dd9616cbe1765d2114b9b3b5c.jpg", "https://fr.web.img6.acsta.net/img/66/da/66da9711dbe0719622ec76dd08a746ec.jpg", "https://fr.web.img6.acsta.net/img/4d/82/4d824f856af71de8e87761ab807379c1.jpg", "https://fr.web.img3.acsta.net/img/8d/0c/8d0cbacd54f7232d0910474e72f81e5a.jpg", "https://fr.web.img6.acsta.net/img/63/eb/63eb9bb6c429b49d6690a8385e891519.jpg", "https://fr.web.img6.acsta.net/img/94/20/9420091c451d50325d2017c2f0a38a61.jpg", "https://fr.web.img2.acsta.net/img/57/60/5760e1b78ff8492f7ab4552753b42c5d.jpg", "https://fr.web.img2.acsta.net/img/a5/06/a506e0414a2370a0aac6f2a5d4309217.jpg", "https://fr.web.img6.acsta.net/pictures/24/02/08/10/01/5798849.jpg"]</t>
+          <t>["https://fr.web.img6.acsta.net/img/6b/da/6bdaeb4a15e035b7aa58b4e87bd47ac7.jpg", "https://fr.web.img2.acsta.net/img/b9/62/b962e3314824b9b32d8cf4320496290c.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>21:15</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Au fil de l'eau</t>
+          <t>Le mystérieux regard du flamant rose</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Diek Grobler</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr"/>
+          <t>Diego Cespedes</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition</t>
+        </is>
+      </c>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>SCOL</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>EauC 3 €</t>
-        </is>
-      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr">
         <is>
-          <t>https://fr.web.img5.acsta.net/c_310_420/img/8c/84/8c84ea614022c2dd45796549199213db.jpg</t>
+          <t>https://fr.web.img5.acsta.net/img/53/64/53648efa9d26840b243a90d1cd2ec989.jpg</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Traverser les plus grands océans du monde, voyager le long d’une rivière ou encore dégringoler du ciel : même la plus minuscule des gouttes d’eau peut vivre de grandes aventures ! Et en chemin, elle peut faire de drôles de rencontres… Des vacanciers qui jouent sur la plage à une petite fille en bateau, en passant par tout un tas de créatures plus étranges les unes que les autres, son voyage ne sera pas de tout repos : une chose est sûre, elle ne restera pas coincée dans un bocal !  Un programme de 5 courts-métrages pour découvrir l’eau sous toutes ses formes qui vous plongera dans des univers aquatiques merveilleux.</t>
+          <t>Début des années 1980, dans le désert chilien. Lidia, 11 ans, grandit au sein d’une famille flamboyante qui a trouvé refuge dans un cabaret, aux abords d’une ville minière. Quand une mystérieuse maladie mortelle commence à se propager, une rumeur affirme qu’elle se transmettrait par un simple regard. La communauté devient rapidement la cible des peurs et fantasmes collectifs. Dans ce western moderne, Lidia défend les siens.</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Animation</t>
+          <t>Drame</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>108</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>France</t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
+          <t>Chile, France, Spain, Belgium, Germany</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Tamara Cortés, Matías Catalán, Paula Dinamarca, Claudia Cabezas, Luis Dubó, Andrés Almeida, Felipe Ríos, Vicente Caballero</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition, Festival de Cannes 2025: Prix Un Certain Regard</t>
+        </is>
+      </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr"/>
+          <t>2025-05-15</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=UscRzx6i53M</t>
+        </is>
+      </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=318158.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=298832.html</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>["https://fr.web.img5.acsta.net/img/0c/3c/0c3cb91629e70dd8efad3ee26e745e77.jpg", "https://fr.web.img6.acsta.net/img/a1/db/a1db8937c2ac49b5b3bae20a36accfd3.jpg", "https://fr.web.img5.acsta.net/img/fe/27/fe27a69a3f9b9969e850b982f0e71422.jpg", "https://fr.web.img6.acsta.net/img/12/7a/127ab85f02cf65f882e1ef1c6cb645b4.jpg", "https://fr.web.img5.acsta.net/img/4e/0e/4e0e47e8b8f5ee30d826259a900506ba.jpg", "https://fr.web.img6.acsta.net/img/5c/c2/5cc22fe2888276b9c8c48602573ce165.jpg", "https://fr.web.img4.acsta.net/img/3e/64/3e64cb84d0c528eb21c266134ccc3344.jpg", "https://fr.web.img5.acsta.net/img/6e/e7/6ee79f8a0cfc96522bf6af877bf956ef.jpg", "https://fr.web.img6.acsta.net/img/f0/7b/f07bd8ce319feedbe596331767acb880.jpg", "https://fr.web.img4.acsta.net/img/83/50/8350059b3e37dcbfc2e3a5ee94caea99.jpg"]</t>
+          <t>["https://fr.web.img2.acsta.net/img/82/90/82907cef76c8a8ed8ab5d99aab91f455.jpg", "https://fr.web.img2.acsta.net/img/44/85/44856197be75652c1527a3fcfc6a3d8b.jpg", "https://fr.web.img4.acsta.net/img/51/ab/51abdf1a07284b46031cdcda424d365e.jpg", "https://fr.web.img3.acsta.net/img/d3/3f/d33f7ebf1c5fefeb979bbd0439b138d0.png"]</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-02-14</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Father, Mother, Sister, Brother</t>
+          <t>Un jour avec mon père</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1896,170 +1921,174 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Jem Jarmusch</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Lion d'or Venise 2025</t>
-        </is>
-      </c>
+          <t>Akinola Davies</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Séance avancée pour jurys - pas dans prog</t>
+        </is>
+      </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>https://fr.web.img6.acsta.net/c_310_420/img/18/de/18decda3afef9ae047694aac0d89c169.jpg</t>
+          <t>https://fr.web.img6.acsta.net/c_310_420/img/3a/17/3a17a236cc7eb6ab8b568027211f5224.jpg</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Father Mother Sister Brother est un long-métrage de fiction en forme de triptyque. Trois histoires qui parlent des relations entre des enfants adultes et leur(s) parent(s) quelque peu distant(s), et aussi des relations entre eux.</t>
+          <t>Un jour avec mon père est un récit semi-autobiographique se déroulant sur une seule journée dans la mégalopole nigériane, Lagos, pendant la crise électorale de 1993. Un père tente de guider ses deux jeunes fils à travers l'immense ville alors que des troubles politiques menacent.</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>Comédie, Drame</t>
+          <t>Drame</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>111</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>United States of America, France, Ireland, Italy, Germany, United Kingdom</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>Tom Waits, Adam Driver, Mayim Bialik, Charlotte Rampling, Cate Blanchett, Vicky Krieps, Sarah Greene, Indya Moore</t>
-        </is>
-      </c>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>Mostra de Venise 2025: Lion d'Or</t>
+          <t>Avant-Première en Compétition, Festival de Cannes 2025: Caméra d'Or - Mention spéciale</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=PA07EmbZ0b0</t>
-        </is>
-      </c>
+          <t>2026-03-25</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=326117.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000019740.html</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>["https://fr.web.img6.acsta.net/img/f0/5b/f05ba2cf29f38c4ae15b0f888e95ae14.jpg", "https://fr.web.img6.acsta.net/img/66/ec/66ece5f954c6eb15009a387ce9864732.jpg", "https://fr.web.img4.acsta.net/img/e7/7c/e77cba675f6327f1873b572ba02f0202.jpg"]</t>
+          <t>["https://fr.web.img2.acsta.net/img/9d/c8/9dc8a396dd653369fa38f649ce901b6c.jpg", "https://fr.web.img4.acsta.net/img/fc/c2/fcc2c65af7e14662b883a61b7ee9c6a4.jpg", "https://fr.web.img6.acsta.net/img/4c/13/4c136a85f4474c6e13b28af2437902c7.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-02-14</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>La femme de ménage</t>
+          <t>Maspalomas</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Paul Feig</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr"/>
+          <t>Aitor Arregi, José Mari Goenaga</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>AP-COMP  Prix Cinema Europa Les Arcs 2025, Prix d'interprétation San Sebastian 2025</t>
+        </is>
+      </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Partenariat Festival DIAM</t>
+        </is>
+      </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>https://fr.web.img3.acsta.net/c_310_420/img/ed/a3/eda3bba832e22c79ea22117b058f84e5.jpg</t>
+          <t>https://fr.web.img5.acsta.net/img/bc/e6/bce6ba592dc6197d53f2b4234b3318b5.jpg</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>En quête d’un nouveau départ, Millie accepte un poste de femme de ménage à demeure chez Nina et Andrew Winchester, un couple aussi riche qu’énigmatique. Ce qui s’annonce comme l’emploi idéal se transforme rapidement en un jeu dangereux, mêlant séduction, secrets et manipulations. Derrière les portes closes du manoir Winchester se cache un monde de faux-semblants et de révélations inattendues… Un tourbillon de suspense et de scandales qui vous tiendra en haleine jusqu’à la dernière seconde.</t>
+          <t>Vicente, un vieil homme ouvertement homosexuel qui, lorsqu'il est admis dans une maison de retraite, décide de cacher son orientation sexuelle.</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>Thriller</t>
+          <t>Drame</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>115</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>United States of America</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Sydney Sweeney, Amanda Seyfried, Brandon Sklenar, Elizabeth Perkins, Michele Morrone, Indiana Elle, Arabella Olivia Clark, Megan Ferguson</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr"/>
+          <t>José Ramón Soroiz, Nagore Aranburu, Kandido Uranga, Zorion Eguileor, Kepa Errasti, Cristina Yélamos, Ana Elordi, Miren Gaztañaga</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>AP-COMP  Prix Cinema Europa Les Arcs 2025, Prix d'interprétation San Sebastian 2025</t>
+        </is>
+      </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-10-06</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=sfdllDBGNzc</t>
+          <t>https://www.youtube.com/watch?v=8o6gkyinORg</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=317403.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000017160.html</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>["https://fr.web.img3.acsta.net/img/f2/dc/f2dcd148cbbb44a015f38bb1c28c1709.jpg", "https://fr.web.img3.acsta.net/img/e7/29/e729e18b103c2087084108af4452eeb9.jpg", "https://fr.web.img5.acsta.net/img/a4/24/a424823bdfc900342ee5a7c4a7af636f.jpg", "https://fr.web.img6.acsta.net/img/d6/7f/d67f20c2f672f2ec9417ca662e52bbed.jpg", "https://fr.web.img4.acsta.net/img/b2/4c/b24c271c8ee9ceb5cd5e0f31ec4acb8c.jpg", "https://fr.web.img6.acsta.net/img/6f/66/6f66c2f4665712fe41c540fba1b8838b.jpg", "https://fr.web.img5.acsta.net/img/91/10/91101a0dd7d81758922c46c0df9cd6a0.jpg", "https://fr.web.img3.acsta.net/img/49/8d/498dc8c1eab1c0cf30a53abbffeffa2c.jpg", "https://fr.web.img5.acsta.net/img/d0/24/d024f3ce64288d52fe496a95b8bc9d27.jpg", "https://fr.web.img3.acsta.net/img/3f/72/3f72a4345de2f1a93dbf8bb3052ba7f4.jpg", "https://fr.web.img4.acsta.net/img/b7/b0/b7b0748d96a509101b6c6e2b0d9749c6.jpg", "https://fr.web.img6.acsta.net/img/6c/78/6c7894999ba2fdb52a7faca437aa8c17.jpg"]</t>
+          <t>["https://fr.web.img6.acsta.net/img/c9/9f/c99f11251f18674fd2b7a422d0691ff8.jpg", "https://fr.web.img3.acsta.net/img/7a/46/7a469765f8608f20460ab2bb2ebca382.jpg", "https://fr.web.img5.acsta.net/img/9e/3a/9e3a25b3bb74c9d42d4690716b5ed194.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-14</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>14:30</t>
+          <t>18:15</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Avatar De feu et de cendres</t>
+          <t>La danse des renards</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2070,79 +2099,91 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>James Cameron</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr"/>
+          <t>Valéry Carnoy</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Repas partagé entres les 2 films 19h45</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>https://fr.web.img5.acsta.net/c_310_420/img/52/fb/52fb8f0345af2b0940557aa049ca19fd.jpg</t>
+          <t>https://fr.web.img5.acsta.net/img/0b/dc/0bdccf730ab568608d09d272f722d91b.jpg</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Le troisième volet de la saga "Avatar".</t>
+          <t>Dans un internat sportif, Camille, un jeune boxeur virtuose, est sauvé in extremis d’un accident mortel par son meilleur ami Matteo. Alors que les médecins le pensent guéri, une douleur inexpliquée l’envahit peu à peu, jusqu’à remettre en question ses rêves de grandeur.</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>Science Fiction, Aventure, Action, Fantastique</t>
+          <t>Drame</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>197</t>
+          <t>90</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>United States of America</t>
+          <t>Belgium, France</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Sam Worthington, Zoe Saldaña, Sigourney Weaver, Stephen Lang, Oona Chaplin, Jack Champion, Kate Winslet, Cliff Curtis</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr"/>
+          <t>Samuel Kircher, Faycal Anaflous, Jef Jacobs, Anna Heckel, Jean-Baptiste Durand, Hassane Alili, Salahdine El Garchi, Yoann Blanc</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition</t>
+        </is>
+      </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-05-17</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Zegl3vxOPjM</t>
+          <t>https://www.youtube.com/watch?v=xdSNIPsLoug</t>
         </is>
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=187247.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=316780.html</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>["https://fr.web.img2.acsta.net/img/61/fc/61fcda398375983affe6f0d5c31bf5b2.jpg", "https://fr.web.img5.acsta.net/img/47/7f/477f5ff3013ca4d5d2d870f92eda682a.jpg", "https://fr.web.img2.acsta.net/img/ea/ae/eaaed8e610626757e3f141b8d999c1f3.jpg", "https://fr.web.img4.acsta.net/img/39/da/39dab8c0535d4e1c299652b2b3481af6.jpg", "https://fr.web.img6.acsta.net/img/23/37/23378b2068f398e80518e2b0b16ac8fb.jpg", "https://fr.web.img4.acsta.net/img/b6/99/b699c77af7fde02081cc37cb8f4dcd5e.jpg", "https://fr.web.img5.acsta.net/img/6d/5d/6d5d367784d2176de109fed0fc8b8f7c.jpg", "https://fr.web.img6.acsta.net/img/af/72/af7276271c7f4684afca337d1c77f7e3.jpg", "https://fr.web.img3.acsta.net/img/12/70/127028875846a08f845c946e48469361.jpg", "https://fr.web.img4.acsta.net/img/49/1a/491afbcfe6ed86a9ffdf780908f7b12f.jpg", "https://fr.web.img6.acsta.net/img/d1/09/d1097323d2d7ac8809c32526cdc988e9.jpg", "https://fr.web.img6.acsta.net/img/fe/29/fe29288e8b4d5e8dcbabe6ec91758110.jpg", "https://fr.web.img2.acsta.net/img/94/45/9445b379cf860c8785f6153c377d7a70.jpg", "https://fr.web.img6.acsta.net/img/83/be/83be72325a1c79e84accfe94d36ace7a.jpg", "https://fr.web.img6.acsta.net/img/94/a1/94a17b292f00e1d5e4cb947f19b9917b.jpg", "https://fr.web.img3.acsta.net/img/e6/8b/e68b4972b506edc94885a1399ddf90da.jpg", "https://fr.web.img2.acsta.net/img/9e/56/9e560702e6396fc060e99fae6cc6f67d.jpg", "https://fr.web.img2.acsta.net/img/08/74/087429d4fb84817496fb83f6815bd079.jpg", "https://fr.web.img6.acsta.net/img/a7/d6/a7d62a13ff7946a061a64c550137e511.jpg", "https://fr.web.img5.acsta.net/img/97/0b/970b1bf6403c59375605784062bbac91.jpg", "https://fr.web.img6.acsta.net/img/47/66/4766a2dff51452fe1bc58fdb89880215.jpg", "https://fr.web.img5.acsta.net/img/28/a7/28a755ef689bd74746b03f9d8773494b.jpg", "https://fr.web.img4.acsta.net/img/d5/71/d5716d5f1aef9ed68e57dd51ea8a0557.jpg", "https://fr.web.img3.acsta.net/img/0e/a2/0ea211356ff9cba35542bf9238ce0064.jpg", "https://fr.web.img2.acsta.net/img/96/4c/964cb2c621023ba74f814a27492e8fdc.jpg", "https://fr.web.img6.acsta.net/img/cc/a2/cca28dc399a8442b8698d2a474290621.jpg", "https://fr.web.img5.acsta.net/img/c5/40/c54097cd49731f0dc5d83e6217caf335.jpg", "https://fr.web.img5.acsta.net/img/4d/17/4d1728ae2058e8e7628e6fc2beed4543.jpg", "https://fr.web.img6.acsta.net/img/ce/85/ce85a7e6bc30a2f0eba463af5d4db097.jpg", "https://fr.web.img4.acsta.net/img/28/07/2807da269b5f9a98b87f7cde2c9df8d7.jpg", "https://fr.web.img3.acsta.net/img/f4/98/f498913ea354447e6bb908398c684148.jpg", "https://fr.web.img6.acsta.net/img/86/8c/868c52cbdd7b829a8dda0242c5b035bc.jpg", "https://fr.web.img6.acsta.net/img/80/99/8099b3ae5d7e42cee546c232f1d2d07a.jpg"]</t>
+          <t>["https://fr.web.img4.acsta.net/img/87/b1/87b13594d74d6a0fe5bc1b5ae98acc87.jpg", "https://fr.web.img5.acsta.net/img/9b/27/9b2717b9517a0b1e09092932b9931850.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-14</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>21:15</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Eleonora Duse</t>
+          <t>Le garçon qui faisait danser les  collines</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2153,83 +2194,71 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Pietro Marcello</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr"/>
+          <t>Georgi M Unkovski</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>Découverte</t>
-        </is>
-      </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr">
         <is>
-          <t>https://fr.web.img3.acsta.net/c_310_420/img/3a/20/3a2040b34e2321ec2db15c025b4ef278.jpg</t>
+          <t>https://fr.web.img6.acsta.net/img/34/e6/34e60dd260546e67f467877cfb5316fc.jpg</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>A la fin de la Première Guerre mondiale, alors que l’Italie enterre son soldat inconnu, la grande Eleonora Duse arrive au terme d’une carrière légendaire. Mais malgré son âge et une santé fragile, celle que beaucoup considèrent comme la plus grande actrice de son époque, décide de remonter sur scène. Les récriminations de sa fille, la relation complexe avec le grand poète D’Annunzio, la montée du fascisme et l’arrivée au pouvoir de Mussolini, rien n’arrêtera Duse "la divine".</t>
+          <t>Ahmet, 15 ans, grandit au milieu des montagnes de Macédoine, où il garde les moutons de son père tout en prenant soin de son petit frère. Mais lui, ce qui le fait rêver, c’est la musique. Entre les attentes de son entourage et ses envies d’ailleurs, Ahmet pourra-t-il un jour suivre son propre chemin ?</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Biopic, Historique</t>
+          <t>Drame, Comédie, Musical</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>Italy, France</t>
-        </is>
-      </c>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>Valeria Bruni Tedeschi, Fanni Wrochna, Noémie Merlant, Fausto Russo Alesi, Edoardo Sorgente, Vincenzo Nemolato, Gaja Masciale, Vincenza Modica</t>
-        </is>
-      </c>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>2026-01-14</t>
-        </is>
-      </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=lTyz6_vxNgA</t>
-        </is>
-      </c>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000004748.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000016927.html</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>["https://fr.web.img3.acsta.net/img/91/86/9186b4fedca51f603f35c489fc40065f.jpg", "https://fr.web.img6.acsta.net/img/e6/af/e6af83e91bcf515ced51bb20b275a013.jpg", "https://fr.web.img3.acsta.net/img/f3/44/f3441deced7205918b66a70ac7572744.jpg", "https://fr.web.img6.acsta.net/img/5f/c5/5fc5e56649395c638772287faf819871.jpg"]</t>
+          <t>["https://fr.web.img4.acsta.net/img/51/fb/51fb8e6064ca7936232006c5e38d7bf9.jpg", "https://fr.web.img3.acsta.net/img/e2/31/e231cd9f9478af56c6927dfe4ca2501b.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-15</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>La pire mère au monde</t>
+          <t>Affection, affection</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2240,31 +2269,35 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Pierre Mazingarbe</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr"/>
+          <t>Alexia Walther, Maxime Matray</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition</t>
+        </is>
+      </c>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
-          <t>https://fr.web.img5.acsta.net/c_310_420/img/ea/fd/eafdfac8bc40d63ec84a32063363565a.jpg</t>
+          <t>https://fr.web.img5.acsta.net/img/b0/82/b082ee3cbe7d6278acd9e6ac39d9d86b.jpg</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Louise de Pileggi, brillante substitut du procureur, a toujours eu des relations compliquées avec sa mère Judith qu’elle n’a pas vue depuis 15 ans. Quand elle se retrouve mutée au petit tribunal où Judith est greffière, Louise devient la cheffe de sa mère. Et pire encore : elles vont devoir collaborer dans une affaire à première vue banale, mais qui va mettre leurs nerfs à vif.</t>
+          <t>Sur la Côte d'Azur, une adolescente disparaît le jour de son anniversaire. Géraldine, employée municipale, s'improvise alors détective. Personne n'a rien vu mais tout le monde a son mot à dire et Géraldine aura du mal à ne pas se laisser submerger par les potins, les théories et les croyances de chacun. Et ce n'est pas le retour inopiné de sa mère qui va lui faciliter la tâche. Une petite ville, c'est bien connu, c'est plein de petits crimes...</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Comédie</t>
+          <t>Comédie dramatique</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>99</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
@@ -2274,35 +2307,31 @@
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Louise Bourgoin, Muriel Robin, Florence Loiret Caille, Sébastien Chassagne, Gustave Kervern, Patrick Descamps, Anne Benoît, Johann Cuny</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr"/>
+          <t>Agathe Bonitzer, Nathalie Richard, Christophe Paou, Marc Susini, Clémentine Kaul-Surdez</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition</t>
+        </is>
+      </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
-        </is>
-      </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=DubZRp9QwsI</t>
-        </is>
-      </c>
+          <t>2025-08-13</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=279638.html</t>
-        </is>
-      </c>
-      <c r="U22" t="inlineStr">
-        <is>
-          <t>["https://fr.web.img4.acsta.net/img/fe/6a/fe6a2d1825f27579b5d5935d1662104f.jpg", "https://fr.web.img3.acsta.net/img/e3/d7/e3d7b58df0f285df881f289cb700433d.jpg", "https://fr.web.img2.acsta.net/img/4a/84/4a844cac98b2225c6a14af1700e6364b.jpg", "https://fr.web.img5.acsta.net/img/0b/e0/0be032fed7ca132697a0236a7442c00d.jpg", "https://fr.web.img2.acsta.net/img/0a/24/0a24e5bb15c4a635d0e3c405676d89b9.jpg", "https://fr.web.img3.acsta.net/img/44/40/444070ee5a8b27c077b983c32e328e95.jpg", "https://fr.web.img6.acsta.net/img/ee/14/ee1484bc856187e7bf54eb4fbc174baf.jpg", "https://fr.web.img5.acsta.net/img/c5/bf/c5bfdaba870ea3b8d87591a083f65456.jpg", "https://fr.web.img6.acsta.net/img/84/69/846975d92773ae0155e3482afb5b4b7f.jpg", "https://fr.web.img2.acsta.net/img/f7/a5/f7a5493041d5a798c783b71a27d026d5.jpg", "https://fr.web.img6.acsta.net/img/5d/b2/5db2f573ff0656b97aff4e839aa30813.jpg", "https://fr.web.img2.acsta.net/img/55/c3/55c32fa89f9070f778c0b90141ff9a1d.jpg", "https://fr.web.img2.acsta.net/img/f0/af/f0af70e4e07ef7f8732123cf6129a461.jpg", "https://fr.web.img5.acsta.net/img/c4/52/c45239fce1251f2373fdec9facf110e0.jpg", "https://fr.web.img4.acsta.net/img/c4/d6/c4d6d97e38ef1575d1183be1e33620bf.jpg", "https://fr.web.img2.acsta.net/img/c5/6c/c56c7f470fc89e634f8c8b8c04da0510.jpg", "https://fr.web.img5.acsta.net/img/b4/13/b4133a66dc6e338546c3df28d75ccf78.jpg"]</t>
-        </is>
-      </c>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000027142.html</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-15</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2312,88 +2341,76 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>La fabrique des monstres</t>
+          <t>Un jour avec mon père</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Steve Hudson</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr"/>
+          <t>Akinola Davies</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>JP</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>TU 4,50 €</t>
-        </is>
-      </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr">
         <is>
-          <t>https://fr.web.img6.acsta.net/c_310_420/img/54/a6/54a6769d8c7f85c019d1b553662355b5.jpg</t>
+          <t>https://fr.web.img6.acsta.net/c_310_420/img/3a/17/3a17a236cc7eb6ab8b568027211f5224.jpg</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Dans le vieux château de Grottegroin, un savant fou fabrique, rafistole et invente sans cesse des monstres farfelus. P'tit Cousu, sa toute première création oubliée avec le temps, sert de guide aux nouveaux monstres. Jusqu’au jour où un cirque débarque en ville… À la recherche d'une nouvelle attraction, son propriétaire Fulbert Montremonstre tente par tous les moyens d'accéder à cette fabrique de monstres. P'tit Cousu pourrait bien être la star de son futur spectacle...</t>
+          <t>Un jour avec mon père est un récit semi-autobiographique se déroulant sur une seule journée dans la mégalopole nigériane, Lagos, pendant la crise électorale de 1993. Un père tente de guider ses deux jeunes fils à travers l'immense ville alors que des troubles politiques menacent.</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Aventure, Animation, Famille, Comédie, Familial</t>
+          <t>Drame</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>92</t>
-        </is>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>Germany, Luxembourg, India, United States of America, United Kingdom</t>
-        </is>
-      </c>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t>Asa Butterfield, Joel Fry, Alison Steadman, Rob Brydon, Seth Usdenov, Fern Brady, Tia Bannon, Jamali Maddix</t>
-        </is>
-      </c>
-      <c r="Q23" t="inlineStr"/>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>Avant-Première en Compétition, Festival de Cannes 2025: Caméra d'Or - Mention spéciale</t>
+        </is>
+      </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
-        </is>
-      </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=SlHrSRmobKQ</t>
-        </is>
-      </c>
+          <t>2026-03-25</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=295622.html</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000019740.html</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>["https://fr.web.img2.acsta.net/img/79/82/7982fc7ff8b63fbfed9918e9b0baa280.jpg", "https://fr.web.img2.acsta.net/img/f6/24/f6249203cf341105a6c68e61c99ec9e9.jpg", "https://fr.web.img3.acsta.net/img/19/51/1951c052b7ce3535741bcd5cd8c0aed3.jpg", "https://fr.web.img5.acsta.net/img/06/28/06284d1f648a1bff82759ccdb6e52e65.jpg", "https://fr.web.img2.acsta.net/img/4d/59/4d5937a65b0e4deb06ef339c13b7fba4.jpg", "https://fr.web.img5.acsta.net/img/f4/23/f4233bb92efba64c87a03525cbb89fa3.jpg", "https://fr.web.img3.acsta.net/img/ae/79/ae792c5b7e618bf71c8bcc4f14861f86.jpg", "https://fr.web.img6.acsta.net/img/95/ac/95ac149ab36d5374c5475c997e44eaac.jpg", "https://fr.web.img2.acsta.net/img/8f/8c/8f8c2968a692b9bfa895227fcb43b85f.jpg"]</t>
+          <t>["https://fr.web.img2.acsta.net/img/9d/c8/9dc8a396dd653369fa38f649ce901b6c.jpg", "https://fr.web.img4.acsta.net/img/fc/c2/fcc2c65af7e14662b883a61b7ee9c6a4.jpg", "https://fr.web.img6.acsta.net/img/4c/13/4c136a85f4474c6e13b28af2437902c7.jpg"]</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-15</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2403,7 +2420,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Qui brille au combat</t>
+          <t>La maison des femmes</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2411,28 +2428,28 @@
           <t>VF</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>CM1</t>
-        </is>
-      </c>
+      <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Joséphine Japy</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr"/>
+          <t>Melisa Godet</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Avant-Première</t>
+        </is>
+      </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr">
         <is>
-          <t>https://fr.web.img6.acsta.net/c_310_420/img/a3/e8/a3e859018636c366010d60f860a255a3.jpg</t>
+          <t>https://fr.web.img5.acsta.net/c_310_420/img/d0/9f/d09ff1ec5ee43c6f7f17d6622d7422d0.jpg</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Qui Brille au Combat est le sens étymologique du prénom Bertille, la plus jeune des deux sœurs de la famille Roussier, atteinte d’un handicap lourd au diagnostic incertain. La famille vit dans un équilibre fragile autour de cet enfant qui accapare les efforts et pensées de chacun, et qui pourrait perdre la vie à tout moment. Chacun se construit, vit comme il peut avec les exigences de ce rythme et les incertitudes qui l’accompagnent. Les parents, Madeleine et Gilles, la sœur aînée, Marion. Quel quotidien et quels avenirs pour une mère, un père, un couple, une adolescente que la responsabilité ​ de sa cadette a rendu trop vite adulte ? Lorsqu’un nouveau diagnostic est posé, les cartes sont rebattues et un nouvel horizon se dessine...</t>
+          <t>À la Maison des femmes, entre soin, écoute et solidarité, une équipe se bat chaque jour pour accompagner les femmes victimes de violences dans leur reconstruction. Dans ce lieu unique, Diane, Manon, Inès, Awa et leurs collègues accueillent, soutiennent, redonnent confiance. Ensemble, avec leurs forces, leurs fragilités, leurs convictions et une énergie inépuisable.</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
@@ -2442,7 +2459,7 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>110</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
@@ -2452,28 +2469,297 @@
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Mélanie Laurent, Pierre-Yves Cardinal, Sarah Pachoud, Angelina Woreth, Félix Kysyl, Stéphane Varupenne, Anne Loiret, Thomas Gioria</t>
-        </is>
-      </c>
-      <c r="Q24" t="inlineStr"/>
+          <t>Karin Viard, Lætitia Dosch, Oulaya Amamra, Eye Haïdara, Pierre Deladonchamps, Juliette Armanet, Laurent Stocker, Jean-Charles Clichet</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>Avant-Première</t>
+        </is>
+      </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-03-04</t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=FbdY7keYTf0</t>
+          <t>https://www.youtube.com/watch?v=yAwvKg9T47Q</t>
         </is>
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000012015.html</t>
-        </is>
-      </c>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>["https://fr.web.img5.acsta.net/img/1c/53/1c5370c57b04620d24ed4561a58e9869.jpg", "https://fr.web.img2.acsta.net/img/17/a8/17a860af580783b6344b88c4a8e59c0b.jpg", "https://fr.web.img2.acsta.net/img/ab/b2/abb23a85af694ee094caca578d1a27bf.jpg", "https://fr.web.img2.acsta.net/img/3c/78/3c78eb8134ba0bae7e6cb0d0866cc7c4.jpg", "https://fr.web.img5.acsta.net/img/68/e8/68e81c3b46a38c56529f7861ac540b8d.jpg", "https://fr.web.img2.acsta.net/img/3b/b7/3bb7dd37c6af3ac447d0bda849149607.jpg"]</t>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000012019.html</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>09:30</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Piro Piro</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>VF</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Sung-ah Min</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>SCOL</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Ec Labastide Clermont</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>https://fr.web.img5.acsta.net/c_310_420/pictures/22/11/25/14/56/2428297.jpg</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Un ensemble de 6 films d’animation poétiques et sensibles où le talent de 2 de jeunes réalisatrices sud coréennes, Baek Miyoung et Min Sung-Ah, dévoile des univers aux couleurs pastel et chaleureuses. Des petits oiseaux tissent le lien entre ces films, dans lesquels on partage des instants de tendresse et d’humour. Programme :Koong ! Flap Flap :Quand un crocodile endormi rencontre un petit oiseau.A bird who loves a flower :L’histoire d’un oiseau qui aimait les fleurs.Ba-Lam :Le parcours initiatique d’un papillon bleu dont l’instinct lui dicte de suivre des fleurs en se laissant porter au gré du vent.Piro Piro :Piro Piro et Dalle sont 2 oiseaux. Le premier vient de la forêt, le second de la ville. Lorsqu’ils se rencontrent devant un magasin de fleurs, Piro Piro voudrait qu’ils s’envolent ensemble vers la forêt mais Dalle ne semble pas en état de voler...Dancing in the rain :Deux lapins dansent sous la pluie.The Newly Coming Seasons :La zone démilitarisée de Corée, créée suite à l’armistice du 27 Juillet 1953, est connue pour être un écosystème intact, loin de toute présence humaine. Mais coups de feux, incendies volontaires et intrusion de plantes étrangères font que de nombreux problèmes persistent entre le Nord et le Sud.</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Animation, Famille</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>SCOL</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>2023-02-01</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=lwkHjaBZSHo</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=307792.html</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>["https://fr.web.img6.acsta.net/pictures/22/09/09/13/04/3096825.jpg", "https://fr.web.img6.acsta.net/pictures/22/09/09/13/04/3081225.jpg", "https://fr.web.img6.acsta.net/pictures/22/09/09/13/03/3533794.jpg", "https://fr.web.img6.acsta.net/pictures/22/09/09/13/03/3519754.jpg", "https://fr.web.img4.acsta.net/pictures/22/09/09/13/03/3505714.jpg", "https://fr.web.img6.acsta.net/pictures/22/09/09/13/03/3491673.jpg", "https://fr.web.img6.acsta.net/pictures/22/09/09/13/03/3477633.jpg", "https://fr.web.img6.acsta.net/pictures/22/09/09/13/03/3463593.jpg", "https://fr.web.img6.acsta.net/pictures/22/09/09/13/03/3449553.jpg", "https://fr.web.img3.acsta.net/pictures/22/09/09/13/03/3433953.jpg", "https://fr.web.img3.acsta.net/pictures/22/09/09/13/03/3419913.jpg", "https://fr.web.img2.acsta.net/pictures/22/09/09/13/03/3404312.jpg"]</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Le mécano de la générale</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>VF</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Clyde Bruckman, Buster Keaton</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>SCOL</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Coll Mandela Noé</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>https://fr.web.img6.acsta.net/c_310_420/pictures/17/05/19/16/07/057072.jpg</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Le cheminot Johnnie Gray partage sa vie entre sa fiancée Annabelle Lee et sa locomotive, la Générale. En pleine Guerre de Sécession, il souhaite s'engager dans l'armée sudiste, mais celle-ci estime qu'il se montrera plus utile en restant mécanicien. Pour prouver à Annabelle qu'il n'est pas lâche, il se lance seul à la poursuite d'espions nordistes qui se sont emparés d'elle et de sa locomotive...</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Action, Comédie</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>United States of America</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Buster Keaton, Marion Mack, Glen Cavender, Jim Farley, Frederick Vroom, Frank Barnes, Charles Henry Smith, Joe Keaton</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>SCOL</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>1927-02-24</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=ZROzVhuddiI</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=108016.html</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>["https://fr.web.img3.acsta.net/medias/nmedia/18/65/53/29/18868528.jpg", "https://fr.web.img3.acsta.net/medias/nmedia/18/65/53/29/18868522.jpg", "https://fr.web.img4.acsta.net/medias/nmedia/18/65/53/29/18868532.jpg", "https://fr.web.img6.acsta.net/medias/nmedia/18/65/53/29/18868526.jpg", "https://fr.web.img3.acsta.net/medias/nmedia/18/65/53/29/18868519.jpg", "https://fr.web.img2.acsta.net/medias/nmedia/18/65/53/29/18868527.jpg", "https://fr.web.img6.acsta.net/medias/nmedia/18/65/53/29/18868517.jpg", "https://fr.web.img5.acsta.net/medias/nmedia/18/65/53/29/18868539.jpg", "https://fr.web.img6.acsta.net/medias/nmedia/18/65/53/29/18868520.jpg", "https://fr.web.img5.acsta.net/medias/nmedia/18/65/53/29/18868308.jpg", "https://fr.web.img4.acsta.net/medias/nmedia/18/65/53/29/18868538.jpg", "https://fr.web.img2.acsta.net/medias/nmedia/18/65/53/29/18868536.jpg", "https://fr.web.img6.acsta.net/medias/nmedia/18/65/53/29/18868534.jpg", "https://fr.web.img4.acsta.net/medias/nmedia/18/65/53/29/18868541.jpg", "https://fr.web.img2.acsta.net/medias/nmedia/18/65/53/29/18868530.jpg", "https://fr.web.img6.acsta.net/pictures/14/04/16/10/34/296957.jpg", "https://fr.web.img4.acsta.net/pictures/14/04/16/10/33/190777.jpg", "https://fr.web.img6.acsta.net/pictures/14/08/08/10/59/411069.jpg", "https://fr.web.img5.acsta.net/pictures/14/04/16/10/35/428400.jpg", "https://fr.web.img2.acsta.net/pictures/14/04/16/10/35/161355.jpg", "https://fr.web.img6.acsta.net/pictures/14/04/16/10/33/563814.jpg", "https://fr.web.img2.acsta.net/pictures/14/04/16/10/32/177456.jpg", "https://fr.web.img5.acsta.net/pictures/210/085/21008581_20130527145850575.jpg", "https://fr.web.img6.acsta.net/pictures/210/085/21008580_20130527145850341.jpg", "https://fr.web.img2.acsta.net/pictures/210/085/21008579_20130527145850106.jpg", "https://fr.web.img3.acsta.net/pictures/210/085/21008578_20130527145849841.jpg", "https://fr.web.img3.acsta.net/medias/nmedia/18/35/20/55/18389120.jpg", "https://fr.web.img4.acsta.net/medias/nmedia/18/35/20/55/18389121.jpg", "https://fr.web.img5.acsta.net/medias/nmedia/18/35/20/55/18389122.jpg", "https://fr.web.img6.acsta.net/medias/nmedia/18/35/20/55/18389123.jpg"]</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>L'affaire Bojarski</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>VF</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>CM2</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Jean-Paul Salomé</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>https://fr.web.img6.acsta.net/c_310_420/img/18/05/18059e8dd9bca2e516d41023cc08d9d1.jpg</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Jan Bojarski, jeune ingénieur polonais, se réfugie en France pendant la guerre. Il y utilise ses dons pour fabriquer des faux papiers pendant l’occupation allemande. Après la guerre, son absence d’état civil l’empêche de déposer les brevets de ses nombreuses inventions et il est limité à des petits boulots mal rémunérés… jusqu’au jour où un gangster lui propose d’utiliser ses talents exceptionnels pour fabriquer des faux billets. Démarre alors pour lui une double vie à l’insu de sa famille. Très vite, il se retrouve dans le viseur de l’inspecteur Mattei, meilleur flic de France.</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>Drame</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>128</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>France, Belgium</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>Reda Kateb, Sara Giraudeau, Bastien Bouillon, Quentin Dolmaire, Pierre Lottin, Camille Japy, Lolita Chammah, Olivier Loustau</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=ArW4d3hKk60</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>https://www.allocine.fr/film/fichefilm_gen_cfilm=1000014092.html</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>["https://fr.web.img4.acsta.net/img/15/d8/15d8fafca4998c253b2513d29f223350.jpg", "https://fr.web.img5.acsta.net/img/81/b3/81b30ddb0cecd137cedc5220f971c839.jpg", "https://fr.web.img6.acsta.net/img/b1/cf/b1cfe81aa1138030e212e9c701898bf6.jpg", "https://fr.web.img5.acsta.net/img/5a/cc/5acce5895b2080afc842c8d57340122c.jpg", "https://fr.web.img6.acsta.net/img/5d/1e/5d1e210d87c5045ba1d443e552d407f3.jpg", "https://fr.web.img6.acsta.net/img/b1/0f/b10f18819f1ccea971de115bc964d1d6.jpg"]</t>
         </is>
       </c>
     </row>

</xml_diff>